<commit_message>
candidate registration excel for batch
</commit_message>
<xml_diff>
--- a/NSDC_Web_Automation/UploadFiles/CandidateRegistration.xlsx
+++ b/NSDC_Web_Automation/UploadFiles/CandidateRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KirtiSingh\Documents\Repository\NSDC_Web_Automation\nsdcregressiontesting\NSDC_Web_Automation\UploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F9FCD8-5474-4ED4-84C2-5C77669F562F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EFB431-ADAD-47B7-BC5D-B4DFA78BAFC4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -486,7 +486,7 @@
     <t>Graduate</t>
   </si>
   <si>
-    <t>Jam</t>
+    <t>Jimmy</t>
   </si>
 </sst>
 </file>

</xml_diff>